<commit_message>
kleine updates voor publicatie
waardelijst 091: waarden voor buismateriaaltype. De waarden voor
buismateriaal zijn nog een grove inventaristie. Deze is nog niet
geharmoniseerd.
</commit_message>
<xml_diff>
--- a/2. objectcatalogus/IMKL2015 v 1.0RC1-object-attributen-ExtraRegels.xlsx
+++ b/2. objectcatalogus/IMKL2015 v 1.0RC1-object-attributen-ExtraRegels.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20400" windowHeight="8325" tabRatio="875" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20400" windowHeight="8325" tabRatio="875" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL2.2ExtraRegels" sheetId="23" state="hidden" r:id="rId1"/>
@@ -2125,9 +2125,6 @@
     <t>eanCode</t>
   </si>
   <si>
-    <t>Doet IMKL2015 niets mee. Nog uitzoeken. nilReason mag.</t>
-  </si>
-  <si>
     <t>Geen extra regels.
 De UOM wordt uitgedrukt via 1 van de volgende OGC URN codes:
 • urn:ogc:def:uom:OGC::m
@@ -2226,6 +2223,9 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>Doet IMKL2015 niets mee. nilReason mag.</t>
   </si>
 </sst>
 </file>
@@ -3560,13 +3560,13 @@
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> 096 19-06-2015 (hoort bij IMKL werkdocument versie 096</a:t>
+            <a:t> 1.0RC1 23-11-2015 (hoort bij IMKL werkdocument versie 1.0RC1</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>UML08</a:t>
+            <a:t>UML1.0RC1</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -3656,7 +3656,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>Er is een kleurcodering om de relevantie en of conditei van een attribuut gebruik aan te geven.</a:t>
+            <a:t>Er is een kleurcodering om de relevantie en of conditie van een attribuut gebruik aan te geven.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3729,7 +3729,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>grijs: optioneel; puur informatief, van minder belang of niet van toepassing (voorbeeld: INSPIRE-attribuut dat niet van toepassing is in KLIP) </a:t>
+            <a:t>grijs: optioneel; puur informatief, van minder belang of niet van toepassing (voorbeeld: INSPIRE-attribuut dat niet van toepassing is in KLICWIN) </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4178,7 +4178,7 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -4279,7 +4279,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="36" customFormat="1" ht="36" customHeight="1">
@@ -4379,7 +4379,7 @@
         <v>131</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1">
@@ -4459,7 +4459,7 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1">
@@ -4579,7 +4579,7 @@
         <v>131</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="4" customFormat="1">
@@ -4599,7 +4599,7 @@
         <v>131</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="1" customFormat="1">
@@ -4619,7 +4619,7 @@
         <v>131</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="13" customFormat="1">
@@ -4659,7 +4659,7 @@
         <v>131</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="13" customFormat="1">
@@ -4862,7 +4862,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="38" customFormat="1" ht="31.5">
@@ -4962,7 +4962,7 @@
         <v>131</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1">
@@ -5042,7 +5042,7 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1">
@@ -5162,7 +5162,7 @@
         <v>131</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="4" customFormat="1">
@@ -5182,7 +5182,7 @@
         <v>131</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1">
@@ -5202,7 +5202,7 @@
         <v>131</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="13" customFormat="1">
@@ -5242,7 +5242,7 @@
         <v>131</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="13" customFormat="1">
@@ -5532,7 +5532,7 @@
         <v>131</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1">
@@ -5612,7 +5612,7 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1">
@@ -5732,7 +5732,7 @@
         <v>131</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="4" customFormat="1">
@@ -5752,7 +5752,7 @@
         <v>131</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1">
@@ -5772,7 +5772,7 @@
         <v>131</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="13" customFormat="1">
@@ -5812,7 +5812,7 @@
         <v>131</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="13" customFormat="1">
@@ -5894,7 +5894,7 @@
         <v>262</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>249</v>
@@ -6043,7 +6043,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1">
@@ -6103,7 +6103,7 @@
         <v>137</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1">
@@ -6123,7 +6123,7 @@
         <v>137</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1">
@@ -6183,7 +6183,7 @@
         <v>131</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="13" customFormat="1">
@@ -6303,7 +6303,7 @@
         <v>131</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1">
@@ -6323,7 +6323,7 @@
         <v>131</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="4" customFormat="1">
@@ -6524,7 +6524,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -6609,7 +6609,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1">
@@ -6769,7 +6769,7 @@
         <v>131</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
@@ -6789,12 +6789,12 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1">
       <c r="A15" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>96</v>
@@ -7085,7 +7085,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1">
@@ -7245,7 +7245,7 @@
         <v>131</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
@@ -7265,12 +7265,12 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1">
       <c r="A15" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>96</v>
@@ -7305,7 +7305,7 @@
         <v>131</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1">
@@ -7574,7 +7574,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1">
@@ -7734,7 +7734,7 @@
         <v>131</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
@@ -7754,12 +7754,12 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1">
       <c r="A15" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>96</v>
@@ -7794,7 +7794,7 @@
         <v>131</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1">
@@ -7834,7 +7834,7 @@
         <v>131</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1">
@@ -8063,7 +8063,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1">
@@ -8203,7 +8203,7 @@
         <v>131</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1">
@@ -8223,12 +8223,12 @@
         <v>131</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>96</v>
@@ -8263,7 +8263,7 @@
         <v>131</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1">
@@ -8303,7 +8303,7 @@
         <v>131</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1">
@@ -8532,7 +8532,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1">
@@ -8672,7 +8672,7 @@
         <v>131</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1">
@@ -8692,12 +8692,12 @@
         <v>131</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>96</v>
@@ -8732,7 +8732,7 @@
         <v>131</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1">
@@ -8772,7 +8772,7 @@
         <v>131</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1">
@@ -8906,7 +8906,9 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
@@ -9005,7 +9007,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1">
@@ -9025,7 +9027,7 @@
         <v>131</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1">
@@ -9045,7 +9047,7 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="64" customFormat="1">
@@ -9163,7 +9165,7 @@
         <v>131</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1">
@@ -9215,8 +9217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -9247,7 +9249,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="42">
       <c r="A1" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -9332,7 +9334,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="61" customFormat="1" ht="76.5" customHeight="1">
@@ -9372,7 +9374,7 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="25" customFormat="1">
@@ -9397,10 +9399,10 @@
     </row>
     <row r="9" spans="1:6" ht="31.5">
       <c r="A9" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>249</v>
@@ -9417,10 +9419,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>249</v>
@@ -9437,10 +9439,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>249</v>
@@ -9452,15 +9454,15 @@
         <v>131</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="31.5">
       <c r="A12" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>249</v>
@@ -9499,7 +9501,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="42">
       <c r="A1" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -9584,7 +9586,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="61" customFormat="1" ht="76.5" customHeight="1">
@@ -9624,7 +9626,7 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="25" customFormat="1">
@@ -9649,10 +9651,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>249</v>
@@ -9669,10 +9671,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>249</v>
@@ -9689,10 +9691,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>249</v>
@@ -9732,7 +9734,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -9817,7 +9819,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1">
@@ -9837,7 +9839,7 @@
         <v>131</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1">
@@ -9857,12 +9859,12 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1">
       <c r="A8" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>195</v>
@@ -9937,7 +9939,7 @@
         <v>131</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="28" customFormat="1">
@@ -9988,7 +9990,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -10073,7 +10075,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1">
@@ -10093,7 +10095,7 @@
         <v>131</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1">
@@ -10113,15 +10115,15 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1">
       <c r="A8" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>249</v>
@@ -10141,7 +10143,7 @@
         <v>203</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>249</v>
@@ -10161,7 +10163,7 @@
         <v>204</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>249</v>
@@ -10181,7 +10183,7 @@
         <v>206</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>249</v>
@@ -10193,7 +10195,7 @@
         <v>131</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="28" customFormat="1">
@@ -10201,7 +10203,7 @@
         <v>136</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>249</v>
@@ -10218,7 +10220,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B13" s="51" t="s">
         <v>195</v>
@@ -10227,13 +10229,13 @@
         <v>249</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E13" s="51" t="s">
         <v>131</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -10253,7 +10255,7 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -10282,7 +10284,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -10367,7 +10369,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="61" customFormat="1" ht="76.5" customHeight="1">
@@ -10407,7 +10409,7 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="25" customFormat="1">
@@ -10432,7 +10434,7 @@
     </row>
     <row r="9" spans="1:6" s="25" customFormat="1">
       <c r="A9" s="25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>195</v>
@@ -10604,7 +10606,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="61" customFormat="1" ht="72.75" customHeight="1">
@@ -10644,7 +10646,7 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="25" customFormat="1">
@@ -10768,7 +10770,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -10813,7 +10815,7 @@
         <v>131</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
@@ -10833,7 +10835,7 @@
         <v>131</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
@@ -10893,12 +10895,12 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>195</v>
@@ -11067,7 +11069,7 @@
         <v>131</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
@@ -11087,7 +11089,7 @@
         <v>131</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
@@ -11147,7 +11149,7 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1">
@@ -11403,7 +11405,7 @@
         <v>131</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
@@ -11423,7 +11425,7 @@
         <v>131</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
@@ -11483,7 +11485,7 @@
         <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1">
@@ -11699,7 +11701,7 @@
         <v>131</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="64" customFormat="1">
@@ -11719,7 +11721,7 @@
         <v>137</v>
       </c>
       <c r="F4" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
@@ -11879,7 +11881,7 @@
         <v>131</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1">
@@ -11899,7 +11901,7 @@
         <v>131</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
@@ -11919,7 +11921,7 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="1" customFormat="1">
@@ -12079,12 +12081,12 @@
         <v>137</v>
       </c>
       <c r="F22" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="51" customFormat="1">
       <c r="A23" s="51" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B23" s="51" t="s">
         <v>195</v>
@@ -12099,7 +12101,7 @@
         <v>137</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -13942,7 +13944,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="63" customFormat="1" ht="62.25" customHeight="1">
@@ -13962,7 +13964,7 @@
         <v>137</v>
       </c>
       <c r="F6" s="72" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="36" customFormat="1" ht="27.75" customHeight="1">
@@ -14002,7 +14004,7 @@
         <v>131</v>
       </c>
       <c r="F8" s="63" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" customHeight="1">
@@ -14209,7 +14211,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -14293,7 +14295,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1">
@@ -14493,7 +14495,9 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
@@ -14507,7 +14511,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -14592,7 +14596,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1">
@@ -14632,7 +14636,7 @@
         <v>137</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1">
@@ -14692,7 +14696,7 @@
         <v>131</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1" ht="31.5">
@@ -14732,7 +14736,7 @@
         <v>137</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>301</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="12" customFormat="1">
@@ -14852,7 +14856,7 @@
         <v>131</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1">
@@ -14872,7 +14876,7 @@
         <v>131</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1">
@@ -15036,7 +15040,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -15481,7 +15485,7 @@
         <v>131</v>
       </c>
       <c r="F23" s="49" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
@@ -15556,7 +15560,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="7"/>
@@ -15601,7 +15605,7 @@
         <v>131</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1">
@@ -15821,7 +15825,7 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1">
@@ -16069,7 +16073,7 @@
         <v>262</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>249</v>
@@ -16650,7 +16654,7 @@
         <v>262</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>249</v>
@@ -17239,7 +17243,7 @@
         <v>262</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>249</v>
@@ -17400,7 +17404,7 @@
         <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1">
@@ -17500,7 +17504,7 @@
         <v>131</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1">
@@ -17580,7 +17584,7 @@
         <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1">
@@ -17720,7 +17724,7 @@
         <v>131</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1">
@@ -17740,7 +17744,7 @@
         <v>131</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="1" customFormat="1">
@@ -17760,7 +17764,7 @@
         <v>131</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="12" customFormat="1">
@@ -17780,7 +17784,7 @@
         <v>131</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="15" customFormat="1">
@@ -17828,7 +17832,7 @@
         <v>262</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>249</v>

</xml_diff>